<commit_message>
chore: adicionar arquivos de teste e ajustes menores
- Adiciona planilha de teste 5º ano
- Atualiza planilha teste 2 anos
- Ajustes de formatação nos arquivos de migração

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/teste 2 anos.xlsx
+++ b/docs/teste 2 anos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUNIELSON\Downloads\Dados SISAM 2025\dados teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUNIELSON\Documents\Project 2026\SISAM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDD6873-2F73-43E7-A269-B8366F8E91B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1181B025-767C-4790-894C-C18347DCCC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>ALUNO</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -563,27 +566,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -605,16 +588,6 @@
         <patternFill>
           <fgColor theme="5" tint="0.39991454817346722"/>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1696,62 +1669,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7E56D75-EB79-4A28-A80F-0F8ADA82847E}" name="Tabela1" displayName="Tabela1" ref="A1:AU2" totalsRowShown="0" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7E56D75-EB79-4A28-A80F-0F8ADA82847E}" name="Tabela1" displayName="Tabela1" ref="A1:AU2" totalsRowShown="0" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:AU2" xr:uid="{A7E56D75-EB79-4A28-A80F-0F8ADA82847E}"/>
   <tableColumns count="47">
-    <tableColumn id="1" xr3:uid="{B2AC6C49-E9E7-4C2A-B657-B53F02F006E4}" name="ANO" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{CBE6B557-24AD-47B2-B92C-1DE287353346}" name="POLO" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{F31680BC-AABF-4069-B10B-C65E8A5FAEC7}" name="ESCOLA" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{68104EC7-48CD-49B5-B34E-58A00B248F12}" name="ALUNO" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{E740304F-1F40-46E8-A591-27E504759FE7}" name="TURMA" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{33BCF94A-4F49-40D6-9FBF-2F2C0B39B824}" name="ANO/SÉRIE" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{BAFD5320-8AE2-4F71-A1DA-45C980D9E950}" name="P/F" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{2BADFF2A-4D14-4223-AF71-ABCDC9B276F3}" name="Q1" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{29ED35CA-9DEC-488A-B0AA-A7F158ABABA5}" name="Q2" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{FF3AD2A6-2FA8-4F3F-A2E0-E3ECB2A0704F}" name="Q3" dataDxfId="44"/>
-    <tableColumn id="11" xr3:uid="{B063A14F-B1E1-4B29-9F17-C431FE3FDE28}" name="Q4" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{B4A66D2C-3E77-4830-B35F-31D6128DD317}" name="Q5" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{7D994210-6054-470A-BAAA-4C1D13E9D213}" name="Q6" dataDxfId="41"/>
-    <tableColumn id="14" xr3:uid="{D4C8C026-7167-406C-9210-E85E9094ABAD}" name="Q7" dataDxfId="40"/>
-    <tableColumn id="15" xr3:uid="{D31BB0E2-9119-4F48-A61F-EC05A92DC018}" name="Q8" dataDxfId="39"/>
-    <tableColumn id="16" xr3:uid="{6852EA79-3AB1-426D-94E1-266379ACA41A}" name="Q9" dataDxfId="38"/>
-    <tableColumn id="17" xr3:uid="{3578B446-D9E0-49B8-AE78-CB0DCFB25D73}" name="Q10" dataDxfId="37"/>
-    <tableColumn id="18" xr3:uid="{816D20D3-50E8-494C-9E81-9C0BB861F8A1}" name="Q11" dataDxfId="36"/>
-    <tableColumn id="19" xr3:uid="{28D2AF30-AEA0-476C-BE2B-851C8356DAB0}" name="Q12" dataDxfId="35"/>
-    <tableColumn id="20" xr3:uid="{C22CB835-9016-4925-93FC-85D91E591EF8}" name="Q13" dataDxfId="34"/>
-    <tableColumn id="21" xr3:uid="{BB34BDBC-0411-42CD-8D80-5A07036B4863}" name="Q14" dataDxfId="33"/>
-    <tableColumn id="22" xr3:uid="{44E294D6-2727-4341-8A5D-B46829203E20}" name="Q15" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{15D00872-A7B2-44CF-8E73-270E5D1DF883}" name="Q16" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{8458FCB7-6543-4030-81C5-6A4AD63CA77B}" name="Q17" dataDxfId="30"/>
-    <tableColumn id="25" xr3:uid="{1F9B5765-703E-4753-BB3A-1182AC17AA4F}" name="Q18" dataDxfId="29"/>
-    <tableColumn id="26" xr3:uid="{E3745FC7-7E52-45BF-955A-878380098D6E}" name="Q19" dataDxfId="28"/>
-    <tableColumn id="27" xr3:uid="{FB6EE26C-3142-413C-8E74-A3350D5E2439}" name="Q20" dataDxfId="27"/>
-    <tableColumn id="28" xr3:uid="{629E3D20-65BF-439D-94E8-6F720EB41073}" name="Q21" dataDxfId="26"/>
-    <tableColumn id="29" xr3:uid="{968E2DC5-525D-492D-BB08-2002267A5212}" name="Q22" dataDxfId="25"/>
-    <tableColumn id="30" xr3:uid="{12013805-BD5E-40BD-8717-496287748BC3}" name="Q23" dataDxfId="24"/>
-    <tableColumn id="31" xr3:uid="{38F359FB-9EAC-44DD-8C32-8A1AC1A8FA7B}" name="Q24" dataDxfId="23"/>
-    <tableColumn id="32" xr3:uid="{32DD316D-427F-4E5E-B543-ECBBC1041585}" name="Q25" dataDxfId="22"/>
-    <tableColumn id="33" xr3:uid="{456D59B8-C692-41BA-9B3E-47D1A3ED1792}" name="Q26" dataDxfId="21"/>
-    <tableColumn id="34" xr3:uid="{AC16C9EA-CF07-4DB1-8859-0AADD622B4D7}" name="Q27" dataDxfId="20"/>
-    <tableColumn id="35" xr3:uid="{C77A6633-ED1D-4F3E-8117-7353FC1A42DC}" name="Q28" dataDxfId="19"/>
-    <tableColumn id="36" xr3:uid="{73166095-14E6-4B36-9D61-EE797CAB8317}" name="Item1" dataDxfId="18"/>
-    <tableColumn id="37" xr3:uid="{E40C0AA0-241D-483D-BF9A-C52085E233DF}" name="Item2" dataDxfId="17"/>
-    <tableColumn id="38" xr3:uid="{40663DA8-A6C5-4659-94D8-BB39ABB778DB}" name="Item3" dataDxfId="16"/>
-    <tableColumn id="39" xr3:uid="{84400F62-318C-44FE-953C-6135B6E6D6CC}" name="Item4" dataDxfId="15"/>
-    <tableColumn id="40" xr3:uid="{9F26704E-E6C6-4270-954A-D6AEE4FF65C2}" name="Item5" dataDxfId="14"/>
-    <tableColumn id="41" xr3:uid="{7C7EA9EC-B835-4570-A71D-26779A9EC5EA}" name="Item6" dataDxfId="13"/>
-    <tableColumn id="42" xr3:uid="{27D1C3CD-78D5-4406-9FAF-3C66ACE00BAB}" name="Item7" dataDxfId="12"/>
-    <tableColumn id="48" xr3:uid="{3EBA68F6-2945-4BD3-A14F-7872E8F75AA8}" name="Item8" dataDxfId="11"/>
-    <tableColumn id="44" xr3:uid="{2A7E0544-F3E9-434D-9776-FF50952A5926}" name="NOTA_LP" dataDxfId="10" dataCellStyle="Vírgula">
+    <tableColumn id="1" xr3:uid="{B2AC6C49-E9E7-4C2A-B657-B53F02F006E4}" name="ANO" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{CBE6B557-24AD-47B2-B92C-1DE287353346}" name="POLO" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{F31680BC-AABF-4069-B10B-C65E8A5FAEC7}" name="ESCOLA" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{68104EC7-48CD-49B5-B34E-58A00B248F12}" name="ALUNO" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{E740304F-1F40-46E8-A591-27E504759FE7}" name="TURMA" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{33BCF94A-4F49-40D6-9FBF-2F2C0B39B824}" name="ANO/SÉRIE" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{BAFD5320-8AE2-4F71-A1DA-45C980D9E950}" name="P/F" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{2BADFF2A-4D14-4223-AF71-ABCDC9B276F3}" name="Q1" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{29ED35CA-9DEC-488A-B0AA-A7F158ABABA5}" name="Q2" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{FF3AD2A6-2FA8-4F3F-A2E0-E3ECB2A0704F}" name="Q3" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{B063A14F-B1E1-4B29-9F17-C431FE3FDE28}" name="Q4" dataDxfId="40"/>
+    <tableColumn id="12" xr3:uid="{B4A66D2C-3E77-4830-B35F-31D6128DD317}" name="Q5" dataDxfId="39"/>
+    <tableColumn id="13" xr3:uid="{7D994210-6054-470A-BAAA-4C1D13E9D213}" name="Q6" dataDxfId="38"/>
+    <tableColumn id="14" xr3:uid="{D4C8C026-7167-406C-9210-E85E9094ABAD}" name="Q7" dataDxfId="37"/>
+    <tableColumn id="15" xr3:uid="{D31BB0E2-9119-4F48-A61F-EC05A92DC018}" name="Q8" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{6852EA79-3AB1-426D-94E1-266379ACA41A}" name="Q9" dataDxfId="35"/>
+    <tableColumn id="17" xr3:uid="{3578B446-D9E0-49B8-AE78-CB0DCFB25D73}" name="Q10" dataDxfId="34"/>
+    <tableColumn id="18" xr3:uid="{816D20D3-50E8-494C-9E81-9C0BB861F8A1}" name="Q11" dataDxfId="33"/>
+    <tableColumn id="19" xr3:uid="{28D2AF30-AEA0-476C-BE2B-851C8356DAB0}" name="Q12" dataDxfId="32"/>
+    <tableColumn id="20" xr3:uid="{C22CB835-9016-4925-93FC-85D91E591EF8}" name="Q13" dataDxfId="31"/>
+    <tableColumn id="21" xr3:uid="{BB34BDBC-0411-42CD-8D80-5A07036B4863}" name="Q14" dataDxfId="30"/>
+    <tableColumn id="22" xr3:uid="{44E294D6-2727-4341-8A5D-B46829203E20}" name="Q15" dataDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{15D00872-A7B2-44CF-8E73-270E5D1DF883}" name="Q16" dataDxfId="28"/>
+    <tableColumn id="24" xr3:uid="{8458FCB7-6543-4030-81C5-6A4AD63CA77B}" name="Q17" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{1F9B5765-703E-4753-BB3A-1182AC17AA4F}" name="Q18" dataDxfId="26"/>
+    <tableColumn id="26" xr3:uid="{E3745FC7-7E52-45BF-955A-878380098D6E}" name="Q19" dataDxfId="25"/>
+    <tableColumn id="27" xr3:uid="{FB6EE26C-3142-413C-8E74-A3350D5E2439}" name="Q20" dataDxfId="24"/>
+    <tableColumn id="28" xr3:uid="{629E3D20-65BF-439D-94E8-6F720EB41073}" name="Q21" dataDxfId="23"/>
+    <tableColumn id="29" xr3:uid="{968E2DC5-525D-492D-BB08-2002267A5212}" name="Q22" dataDxfId="22"/>
+    <tableColumn id="30" xr3:uid="{12013805-BD5E-40BD-8717-496287748BC3}" name="Q23" dataDxfId="21"/>
+    <tableColumn id="31" xr3:uid="{38F359FB-9EAC-44DD-8C32-8A1AC1A8FA7B}" name="Q24" dataDxfId="20"/>
+    <tableColumn id="32" xr3:uid="{32DD316D-427F-4E5E-B543-ECBBC1041585}" name="Q25" dataDxfId="19"/>
+    <tableColumn id="33" xr3:uid="{456D59B8-C692-41BA-9B3E-47D1A3ED1792}" name="Q26" dataDxfId="18"/>
+    <tableColumn id="34" xr3:uid="{AC16C9EA-CF07-4DB1-8859-0AADD622B4D7}" name="Q27" dataDxfId="17"/>
+    <tableColumn id="35" xr3:uid="{C77A6633-ED1D-4F3E-8117-7353FC1A42DC}" name="Q28" dataDxfId="16"/>
+    <tableColumn id="36" xr3:uid="{73166095-14E6-4B36-9D61-EE797CAB8317}" name="Item1" dataDxfId="15"/>
+    <tableColumn id="37" xr3:uid="{E40C0AA0-241D-483D-BF9A-C52085E233DF}" name="Item2" dataDxfId="14"/>
+    <tableColumn id="38" xr3:uid="{40663DA8-A6C5-4659-94D8-BB39ABB778DB}" name="Item3" dataDxfId="13"/>
+    <tableColumn id="39" xr3:uid="{84400F62-318C-44FE-953C-6135B6E6D6CC}" name="Item4" dataDxfId="12"/>
+    <tableColumn id="40" xr3:uid="{9F26704E-E6C6-4270-954A-D6AEE4FF65C2}" name="Item5" dataDxfId="11"/>
+    <tableColumn id="41" xr3:uid="{7C7EA9EC-B835-4570-A71D-26779A9EC5EA}" name="Item6" dataDxfId="10"/>
+    <tableColumn id="42" xr3:uid="{27D1C3CD-78D5-4406-9FAF-3C66ACE00BAB}" name="Item7" dataDxfId="9"/>
+    <tableColumn id="48" xr3:uid="{3EBA68F6-2945-4BD3-A14F-7872E8F75AA8}" name="Item8" dataDxfId="8"/>
+    <tableColumn id="44" xr3:uid="{2A7E0544-F3E9-434D-9776-FF50952A5926}" name="NOTA_LP" dataDxfId="7" dataCellStyle="Vírgula">
       <calculatedColumnFormula>IF(D2="","-",COUNTIF(H2:U2,"X"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{1DC73ABF-C9F2-4931-8CFB-A801B5125F66}" name="NOTA_MAT" dataDxfId="9" dataCellStyle="Vírgula">
+    <tableColumn id="45" xr3:uid="{1DC73ABF-C9F2-4931-8CFB-A801B5125F66}" name="NOTA_MAT" dataDxfId="6" dataCellStyle="Vírgula">
       <calculatedColumnFormula>IF(D2="","-",COUNTIF(V2:AI2,"X"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{E1C8680E-2A02-489E-A3B1-E6C7E3AA3E9B}" name="PRODUÇÃO" dataDxfId="8" dataCellStyle="Vírgula">
+    <tableColumn id="46" xr3:uid="{E1C8680E-2A02-489E-A3B1-E6C7E3AA3E9B}" name="PRODUÇÃO" dataDxfId="5" dataCellStyle="Vírgula">
       <calculatedColumnFormula>IF(D2="","-",COUNTIF(AJ2:AP2,"X"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{8EEE2E5D-B220-4B4D-98F7-657CDA4FA3B4}" name="NÍVEL_PROD" dataDxfId="7" dataCellStyle="Vírgula">
+    <tableColumn id="47" xr3:uid="{8EEE2E5D-B220-4B4D-98F7-657CDA4FA3B4}" name="NÍVEL_PROD" dataDxfId="4" dataCellStyle="Vírgula">
       <calculatedColumnFormula>IF(AT2="","-",IF(AT2=0,"S/R",IF(AT2&lt;3,"N1",IF(AT2&lt;=5,"N2",IF(AT2&lt;=7,"N3",IF(AT2="-","-","N4"))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2028,7 +2001,7 @@
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AT9" sqref="AT9"/>
+      <selection activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2296,9 +2269,7 @@
       <c r="AJ2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="AK2" s="6"/>
       <c r="AL2" s="6" t="s">
         <v>54</v>
       </c>
@@ -2306,14 +2277,12 @@
         <v>54</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP2" s="6" t="s">
-        <v>55</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="AP2" s="6"/>
       <c r="AQ2" s="29" t="s">
         <v>54</v>
       </c>
@@ -2336,17 +2305,17 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H2:AQ2">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",H2)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
chore: adicionar scripts auxiliares e documentação
Scripts:
- migrate-divergencias-historico.js: migration para tabela de histórico
- verificar-dados-orfaos.ts: verificação de dados órfãos
- verificar-dados-questoes.ts: verificação de questões
- verificar-questoes-por-serie.ts: questões por série
- verificar-correcao-cascade.ts: verificar correções em cascade
- executar-migration-cascade.ts: executar migrations
- debug-relatorio.ts: debug de relatórios
- testar-dados-relatorio.ts: testes de dados
- atualizar-layouts-admin.ts: atualização de layouts

Documentação:
- RELATORIOS_PDF_IMPLEMENTACAO.md: docs do sistema de relatórios
- Atualizações em docs de configuração Vercel

API:
- debug-relatorio/route.ts: endpoint para debug

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/teste 2 anos.xlsx
+++ b/docs/teste 2 anos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUNIELSON\Documents\Project 2026\SISAM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1181B025-767C-4790-894C-C18347DCCC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F55AEC-1FB9-47F2-BD2C-26FFEA0B3597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2º Ano e 3º Ano " sheetId="6" r:id="rId1"/>
@@ -1722,7 +1722,7 @@
       <calculatedColumnFormula>IF(D2="","-",COUNTIF(V2:AI2,"X"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="46" xr3:uid="{E1C8680E-2A02-489E-A3B1-E6C7E3AA3E9B}" name="PRODUÇÃO" dataDxfId="5" dataCellStyle="Vírgula">
-      <calculatedColumnFormula>IF(D2="","-",COUNTIF(AJ2:AP2,"X"))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(D2="","-",COUNTIF(AJ2:AQ2,"X"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="47" xr3:uid="{8EEE2E5D-B220-4B4D-98F7-657CDA4FA3B4}" name="NÍVEL_PROD" dataDxfId="4" dataCellStyle="Vírgula">
       <calculatedColumnFormula>IF(AT2="","-",IF(AT2=0,"S/R",IF(AT2&lt;3,"N1",IF(AT2&lt;=5,"N2",IF(AT2&lt;=7,"N3",IF(AT2="-","-","N4"))))))</calculatedColumnFormula>
@@ -2001,7 +2001,7 @@
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+      <selection activeCell="AT12" sqref="AT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2295,12 +2295,12 @@
         <v>12</v>
       </c>
       <c r="AT2" s="8">
-        <f t="shared" ref="AT2" si="2">IF(D2="","-",COUNTIF(AJ2:AP2,"X"))</f>
-        <v>5</v>
+        <f>IF(D2="","-",COUNTIF(AJ2:AQ2,"X"))</f>
+        <v>6</v>
       </c>
       <c r="AU2" s="11" t="str">
         <f>IF(AT2="","-",IF(AT2=0,"S/R",IF(AT2&lt;3,"N1",IF(AT2&lt;=5,"N2",IF(AT2&lt;=7,"N3",IF(AT2="-","-","N4"))))))</f>
-        <v>N2</v>
+        <v>N3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>